<commit_message>
init projet angular + manyToOne membre/pirate et navire/bateau
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20100\Dev\POEI_Sopra\UnePiece\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F090E1-E051-43A1-B1EC-7B886039B135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8874E912-C22B-4B71-8B4B-648F08994C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="1440" windowWidth="28440" windowHeight="17235" xr2:uid="{CE1E904A-62A0-485B-AD72-3207D5E1DE30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CE1E904A-62A0-485B-AD72-3207D5E1DE30}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>activités utilisateur</t>
   </si>
   <si>
-    <t>page parties</t>
-  </si>
-  <si>
     <t>lancer nouvelle partie</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>après trajet : rediriger vers ile destination</t>
+  </si>
+  <si>
+    <t>accueil joueur</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -488,26 +488,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -831,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCAE3EB-9410-42D9-92BE-5BDF53EB6848}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,16 +910,16 @@
         <v>1</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>41</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -935,169 +932,152 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="20"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="25"/>
+      <c r="F14" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>40</v>
+      <c r="D15" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="20"/>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>38</v>
+      <c r="E16" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="20"/>
-      <c r="C17" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>48</v>
+      <c r="C17" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="20"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="30" t="s">
-        <v>47</v>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="20"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>74</v>
+      <c r="D19" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="20"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>75</v>
+      <c r="F20" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="20"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="25"/>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="24"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="20"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="25"/>
+      <c r="F22" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="24"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="25"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="37"/>
+      <c r="G24" s="34"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1109,111 +1089,111 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>